<commit_message>
prepare for ecta submission
</commit_message>
<xml_diff>
--- a/Tables/consort.xlsx
+++ b/Tables/consort.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653878F0-B486-4E69-A862-410556D8FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE37DFF-6E76-4E48-B45E-018E7A5DD055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="2955" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp_arms" sheetId="1" r:id="rId1"/>
     <sheet name="consort" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">consort!$B$2:$I$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">consort!$B$2:$I$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -296,15 +296,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>34925</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -318,9 +318,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="568325" y="663575"/>
-          <a:ext cx="9525" cy="3556000"/>
+        <a:xfrm flipH="1">
+          <a:off x="546100" y="673100"/>
+          <a:ext cx="15875" cy="3790950"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -981,8 +981,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="838198" y="1311275"/>
-          <a:ext cx="209552" cy="631824"/>
+          <a:off x="860423" y="1298575"/>
+          <a:ext cx="209552" cy="628649"/>
           <a:chOff x="1047750" y="1435100"/>
           <a:chExt cx="0" cy="1857375"/>
         </a:xfrm>
@@ -1105,8 +1105,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="952499" y="1311276"/>
-          <a:ext cx="142876" cy="631824"/>
+          <a:off x="974724" y="1298576"/>
+          <a:ext cx="142876" cy="628649"/>
           <a:chOff x="1047750" y="1435100"/>
           <a:chExt cx="0" cy="1857375"/>
         </a:xfrm>
@@ -1229,8 +1229,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1333500" y="1311275"/>
-          <a:ext cx="0" cy="2124075"/>
+          <a:off x="1355725" y="1298575"/>
+          <a:ext cx="0" cy="2111375"/>
           <a:chOff x="1047750" y="1435100"/>
           <a:chExt cx="0" cy="1857375"/>
         </a:xfrm>
@@ -1353,8 +1353,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1447800" y="1311275"/>
-          <a:ext cx="0" cy="2124075"/>
+          <a:off x="1498600" y="1298575"/>
+          <a:ext cx="0" cy="2111375"/>
           <a:chOff x="1047750" y="1435100"/>
           <a:chExt cx="0" cy="1857375"/>
         </a:xfrm>
@@ -1477,8 +1477,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1539875" y="1311275"/>
-          <a:ext cx="0" cy="2124075"/>
+          <a:off x="1609725" y="1298575"/>
+          <a:ext cx="0" cy="2111375"/>
           <a:chOff x="1047750" y="1435100"/>
           <a:chExt cx="0" cy="1857375"/>
         </a:xfrm>
@@ -1601,8 +1601,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1695450" y="1314450"/>
-          <a:ext cx="171450" cy="2124075"/>
+          <a:off x="1765300" y="1301750"/>
+          <a:ext cx="187325" cy="2111375"/>
           <a:chOff x="1047750" y="1435100"/>
           <a:chExt cx="0" cy="1857375"/>
         </a:xfrm>
@@ -1920,8 +1920,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1101725" y="3908424"/>
-          <a:ext cx="190500" cy="434973"/>
+          <a:off x="1123950" y="3876674"/>
+          <a:ext cx="190500" cy="447673"/>
           <a:chOff x="1047750" y="1435100"/>
           <a:chExt cx="0" cy="1857375"/>
         </a:xfrm>
@@ -2385,43 +2385,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDDCAD2-19B6-4E14-AFEE-A572D35A857A}">
   <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="5" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F6" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0.9710926016658501</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>5</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>19246</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>22064</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <f>B23+21916</f>
         <v>41162</v>
@@ -2554,7 +2554,7 @@
         <v>43980</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C26">
         <f>C23-B23</f>
         <v>102</v>
@@ -2580,26 +2580,26 @@
   </sheetPr>
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="6" max="6" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="1.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="2:10" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="19" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -2621,7 +2621,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B4" s="19">
         <f>exp_arms!D24</f>
         <v>41123</v>
@@ -2636,7 +2636,7 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="2:10" ht="5.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="5.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="15"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -2647,7 +2647,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="2:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="19">
         <f>exp_arms!B24</f>
         <v>41162</v>
@@ -2664,7 +2664,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="2:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="16"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -2674,7 +2674,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="16"/>
       <c r="C8" s="7"/>
       <c r="E8" s="7"/>
@@ -2687,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B9" s="16"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -2697,7 +2697,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="16"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -2713,7 +2713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="8.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="16"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -2723,7 +2723,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B12" s="16"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -2744,7 +2744,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -2765,7 +2765,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B14" s="16"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -2785,7 +2785,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B15" s="16"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -2806,7 +2806,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B16" s="16"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2816,7 +2816,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B17" s="19">
         <f>exp_arms!C24</f>
         <v>41264</v>
@@ -2831,7 +2831,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="2:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="24.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="19"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2841,7 +2841,7 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="2:10" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="9.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="15"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2852,7 +2852,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B20" s="19">
         <f>exp_arms!E24</f>
         <v>41499</v>
@@ -2867,7 +2867,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="16"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -2877,7 +2877,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2895,7 +2895,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="11" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="11" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>